<commit_message>
update bom to unclude mfg#
</commit_message>
<xml_diff>
--- a/export/roPlug-BOM.xlsx
+++ b/export/roPlug-BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
+    <t xml:space="preserve">MFG Part#</t>
+  </si>
+  <si>
     <t xml:space="preserve">SW1</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t xml:space="preserve">ATmega32U4-MU</t>
   </si>
   <si>
+    <t xml:space="preserve">ATMEGA32U4-MU</t>
+  </si>
+  <si>
     <t xml:space="preserve">P1</t>
   </si>
   <si>
@@ -79,6 +85,9 @@
     <t xml:space="preserve">USB_C_Plug</t>
   </si>
   <si>
+    <t xml:space="preserve">USB4155-03-C </t>
+  </si>
+  <si>
     <t xml:space="preserve">Y1</t>
   </si>
   <si>
@@ -88,18 +97,30 @@
     <t xml:space="preserve">16MHz</t>
   </si>
   <si>
+    <t xml:space="preserve">EB3250YA12-16.000M (alternative)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA534160F35HDT</t>
+  </si>
+  <si>
     <t xml:space="preserve">R5,R4,R2,R1</t>
   </si>
   <si>
     <t xml:space="preserve">R_0603_1608Metric</t>
   </si>
   <si>
+    <t xml:space="preserve">CRG0603F22R </t>
+  </si>
+  <si>
     <t xml:space="preserve">R3</t>
   </si>
   <si>
     <t xml:space="preserve">10k</t>
   </si>
   <si>
+    <t xml:space="preserve">CPF0603B10KE </t>
+  </si>
+  <si>
     <t xml:space="preserve">F1</t>
   </si>
   <si>
@@ -109,6 +130,9 @@
     <t xml:space="preserve">500mA</t>
   </si>
   <si>
+    <t xml:space="preserve">CC12H500mA-TR </t>
+  </si>
+  <si>
     <t xml:space="preserve">C7,C5,C2,C1</t>
   </si>
   <si>
@@ -118,16 +142,25 @@
     <t xml:space="preserve">0.1uF</t>
   </si>
   <si>
+    <t xml:space="preserve">GRM033R61A104ME15J </t>
+  </si>
+  <si>
     <t xml:space="preserve">C6</t>
   </si>
   <si>
     <t xml:space="preserve">1uF</t>
   </si>
   <si>
+    <t xml:space="preserve">GRM033R60J105MEA2J </t>
+  </si>
+  <si>
     <t xml:space="preserve">C4,C3</t>
   </si>
   <si>
     <t xml:space="preserve">22pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM0335C1H220JA01J </t>
   </si>
 </sst>
 </file>
@@ -142,6 +175,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -223,20 +257,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -261,22 +297,25 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
@@ -287,16 +326,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
@@ -307,16 +346,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,16 +366,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -341,16 +386,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -358,16 +409,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>22</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,16 +429,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -392,16 +449,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,16 +469,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,16 +489,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>33</v>
+        <v>42</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,16 +509,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>